<commit_message>
new excel file new gantt chart based on new targets
</commit_message>
<xml_diff>
--- a/deliverables/ganttChartAvocadoBudget_V3.xlsx
+++ b/deliverables/ganttChartAvocadoBudget_V3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielcronauer/Desktop/ceg4110-group-project-avocadobudget/deliverables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5B5FD1F-0B8C-964E-94EF-51F4EDE27FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788ECB41-1FDD-E648-A6D9-9517B1CBBB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{AB48C4DA-0DA3-C24A-B5FB-8C34E6C351BB}"/>
+    <workbookView xWindow="30240" yWindow="-4900" windowWidth="25960" windowHeight="19080" activeTab="2" xr2:uid="{AB48C4DA-0DA3-C24A-B5FB-8C34E6C351BB}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChartGraph" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="43">
   <si>
     <t>Team Composition Form</t>
   </si>
@@ -167,6 +167,12 @@
   </si>
   <si>
     <t>Expected End Date</t>
+  </si>
+  <si>
+    <t>Design Specification</t>
+  </si>
+  <si>
+    <t>Crud Operations</t>
   </si>
 </sst>
 </file>
@@ -2015,22 +2021,22 @@
                   <c:v>Wireframe</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>Design Specification</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Table Design</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>Design Specificaition</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>CRUD operations</c:v>
+                  <c:v>UI Tasks Complete</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>UI Tasks Complete</c:v>
+                  <c:v>HTML / CSS - Finailzed</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Business Logic / Code complete</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>HTML / CSS - Finailzed</c:v>
+                  <c:v>Crud Operations</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Reports - integrate for reports</c:v>
@@ -2069,19 +2075,19 @@
                   <c:v>45557</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45557</c:v>
+                  <c:v>45562</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45551</c:v>
+                  <c:v>45562</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45562</c:v>
+                  <c:v>45576</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45565</c:v>
+                  <c:v>45576</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45564</c:v>
+                  <c:v>41923</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>45579</c:v>
@@ -2090,7 +2096,7 @@
                   <c:v>45579</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>45593</c:v>
+                  <c:v>45595</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>45600</c:v>
@@ -2150,22 +2156,22 @@
                   <c:v>Wireframe</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>Design Specification</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Table Design</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>Design Specificaition</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>CRUD operations</c:v>
+                  <c:v>UI Tasks Complete</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>UI Tasks Complete</c:v>
+                  <c:v>HTML / CSS - Finailzed</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Business Logic / Code complete</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>HTML / CSS - Finailzed</c:v>
+                  <c:v>Crud Operations</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Reports - integrate for reports</c:v>
@@ -2207,25 +2213,25 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>14</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>7</c:v>
@@ -2520,22 +2526,22 @@
                   <c:v>Wireframe</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>Design Specification</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Table Design</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>Design Specificaition</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>CRUD operations</c:v>
+                  <c:v>UI Tasks Complete</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>UI Tasks Complete</c:v>
+                  <c:v>HTML / CSS - Finailzed</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Business Logic / Code complete</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>HTML / CSS - Finailzed</c:v>
+                  <c:v>Crud Operations</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Reports - integrate for reports</c:v>
@@ -2574,19 +2580,19 @@
                   <c:v>45557</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45557</c:v>
+                  <c:v>45562</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45551</c:v>
+                  <c:v>45562</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45562</c:v>
+                  <c:v>45576</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45565</c:v>
+                  <c:v>45576</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45564</c:v>
+                  <c:v>41923</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>45579</c:v>
@@ -2595,7 +2601,7 @@
                   <c:v>45579</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>45593</c:v>
+                  <c:v>45595</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>45600</c:v>
@@ -2663,22 +2669,22 @@
                   <c:v>Wireframe</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>Design Specification</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Table Design</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>Design Specificaition</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>CRUD operations</c:v>
+                  <c:v>UI Tasks Complete</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>UI Tasks Complete</c:v>
+                  <c:v>HTML / CSS - Finailzed</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Business Logic / Code complete</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>HTML / CSS - Finailzed</c:v>
+                  <c:v>Crud Operations</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Reports - integrate for reports</c:v>
@@ -2717,25 +2723,25 @@
                   <c:v>45562</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45571</c:v>
+                  <c:v>45576</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45572</c:v>
+                  <c:v>45576</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45576</c:v>
+                  <c:v>45579</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45579</c:v>
+                  <c:v>45583</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45578</c:v>
+                  <c:v>41933</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>45593</c:v>
+                  <c:v>45595</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>45593</c:v>
+                  <c:v>45595</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>45600</c:v>
@@ -6213,7 +6219,7 @@
   </sheetPr>
   <dimension ref="N15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
@@ -7956,8 +7962,8 @@
   </sheetPr>
   <dimension ref="A1:X103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8318,12 +8324,11 @@
         <v>25</v>
       </c>
       <c r="F8" s="8">
-        <f t="shared" si="1"/>
-        <v>45557</v>
+        <v>45562</v>
       </c>
       <c r="G8" s="8">
         <f t="shared" si="2"/>
-        <v>45571</v>
+        <v>45576</v>
       </c>
       <c r="H8" s="9">
         <v>14</v>
@@ -8362,18 +8367,17 @@
         <v>35</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="F9" s="8">
-        <f t="shared" si="1"/>
-        <v>45551</v>
+        <v>45562</v>
       </c>
       <c r="G9" s="8">
         <f t="shared" si="2"/>
-        <v>45572</v>
+        <v>45576</v>
       </c>
       <c r="H9" s="9">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I9" s="5">
         <v>9</v>
@@ -8409,19 +8413,17 @@
         <v>46</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F10" s="8">
-        <f t="shared" si="1"/>
-        <v>45562</v>
+        <v>45576</v>
       </c>
       <c r="G10" s="8">
         <f t="shared" si="2"/>
-        <v>45576</v>
+        <v>45579</v>
       </c>
       <c r="H10" s="9">
-        <f t="shared" si="3"/>
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="I10" s="5">
         <v>10</v>
@@ -8457,19 +8459,17 @@
         <v>49</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F11" s="8">
-        <f t="shared" si="1"/>
-        <v>45565</v>
+        <v>45576</v>
       </c>
       <c r="G11" s="8">
         <f t="shared" si="2"/>
-        <v>45579</v>
+        <v>45583</v>
       </c>
       <c r="H11" s="9">
-        <f t="shared" si="3"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="I11" s="5">
         <v>11</v>
@@ -8505,19 +8505,17 @@
         <v>48</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F12" s="8">
-        <f t="shared" si="1"/>
-        <v>45564</v>
+        <v>41923</v>
       </c>
       <c r="G12" s="8">
         <f t="shared" si="2"/>
-        <v>45578</v>
+        <v>41933</v>
       </c>
       <c r="H12" s="9">
-        <f t="shared" si="3"/>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I12" s="5">
         <v>12</v>
@@ -8555,11 +8553,10 @@
       </c>
       <c r="G13" s="8">
         <f t="shared" si="2"/>
-        <v>45593</v>
+        <v>45595</v>
       </c>
       <c r="H13" s="9">
-        <f t="shared" si="3"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I13" s="5">
         <v>13</v>
@@ -8586,7 +8583,7 @@
         <v>63</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F14" s="8">
         <f t="shared" si="1"/>
@@ -8594,11 +8591,10 @@
       </c>
       <c r="G14" s="8">
         <f t="shared" si="2"/>
-        <v>45593</v>
+        <v>45595</v>
       </c>
       <c r="H14" s="9">
-        <f t="shared" si="3"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I14" s="5">
         <v>14</v>
@@ -8628,16 +8624,14 @@
         <v>32</v>
       </c>
       <c r="F15" s="8">
-        <f t="shared" si="1"/>
-        <v>45593</v>
+        <v>45595</v>
       </c>
       <c r="G15" s="8">
         <f t="shared" si="2"/>
         <v>45600</v>
       </c>
       <c r="H15" s="9">
-        <f t="shared" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I15" s="5">
         <v>15</v>
@@ -8996,7 +8990,8 @@
         <v>45562</v>
       </c>
     </row>
-    <row r="33" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E33" s="2"/>
       <c r="I33" s="5">
         <v>33</v>
       </c>
@@ -9007,7 +9002,7 @@
         <v>45563</v>
       </c>
     </row>
-    <row r="34" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="5:11" x14ac:dyDescent="0.2">
       <c r="I34" s="5">
         <v>34</v>
       </c>
@@ -9018,7 +9013,7 @@
         <v>45564</v>
       </c>
     </row>
-    <row r="35" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="5:11" x14ac:dyDescent="0.2">
       <c r="I35" s="5">
         <v>35</v>
       </c>
@@ -9029,7 +9024,7 @@
         <v>45565</v>
       </c>
     </row>
-    <row r="36" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="5:11" x14ac:dyDescent="0.2">
       <c r="I36" s="5">
         <v>36</v>
       </c>
@@ -9040,7 +9035,7 @@
         <v>45566</v>
       </c>
     </row>
-    <row r="37" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="5:11" x14ac:dyDescent="0.2">
       <c r="I37" s="5">
         <v>37</v>
       </c>
@@ -9051,7 +9046,7 @@
         <v>45567</v>
       </c>
     </row>
-    <row r="38" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="5:11" x14ac:dyDescent="0.2">
       <c r="I38" s="5">
         <v>38</v>
       </c>
@@ -9062,7 +9057,7 @@
         <v>45568</v>
       </c>
     </row>
-    <row r="39" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="5:11" x14ac:dyDescent="0.2">
       <c r="I39" s="5">
         <v>39</v>
       </c>
@@ -9073,7 +9068,7 @@
         <v>45569</v>
       </c>
     </row>
-    <row r="40" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="5:11" x14ac:dyDescent="0.2">
       <c r="I40" s="5">
         <v>40</v>
       </c>
@@ -9084,7 +9079,7 @@
         <v>45570</v>
       </c>
     </row>
-    <row r="41" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="5:11" x14ac:dyDescent="0.2">
       <c r="I41" s="5">
         <v>41</v>
       </c>
@@ -9095,7 +9090,7 @@
         <v>45571</v>
       </c>
     </row>
-    <row r="42" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="5:11" x14ac:dyDescent="0.2">
       <c r="I42" s="5">
         <v>42</v>
       </c>
@@ -9106,7 +9101,7 @@
         <v>45572</v>
       </c>
     </row>
-    <row r="43" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="5:11" x14ac:dyDescent="0.2">
       <c r="I43" s="5">
         <v>43</v>
       </c>
@@ -9117,7 +9112,7 @@
         <v>45573</v>
       </c>
     </row>
-    <row r="44" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="5:11" x14ac:dyDescent="0.2">
       <c r="I44" s="5">
         <v>44</v>
       </c>
@@ -9128,7 +9123,7 @@
         <v>45574</v>
       </c>
     </row>
-    <row r="45" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="5:11" x14ac:dyDescent="0.2">
       <c r="I45" s="5">
         <v>45</v>
       </c>
@@ -9139,7 +9134,7 @@
         <v>45575</v>
       </c>
     </row>
-    <row r="46" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="5:11" x14ac:dyDescent="0.2">
       <c r="I46" s="5">
         <v>46</v>
       </c>
@@ -9150,7 +9145,7 @@
         <v>45576</v>
       </c>
     </row>
-    <row r="47" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="5:11" x14ac:dyDescent="0.2">
       <c r="I47" s="5">
         <v>47</v>
       </c>
@@ -9161,7 +9156,7 @@
         <v>45577</v>
       </c>
     </row>
-    <row r="48" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="5:11" x14ac:dyDescent="0.2">
       <c r="I48" s="5">
         <v>48</v>
       </c>

</xml_diff>